<commit_message>
More tests for Persons obj.
</commit_message>
<xml_diff>
--- a/test/data/test_departments.xlsx
+++ b/test/data/test_departments.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jof/Source/bordsplacering/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC493C29-C5C9-9941-8999-6A0BF3B32381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{702226F9-E703-4549-92B0-91B27F1E84C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16840" xr2:uid="{43237B51-ED5E-0440-8A60-CA3551BB0D7F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="test_departments" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -59,9 +59,6 @@
     <t>Maint</t>
   </si>
   <si>
-    <t>Mantainence</t>
-  </si>
-  <si>
     <t>Mechanic</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Synonyms…</t>
+  </si>
+  <si>
+    <t>Maintainence</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,10 +482,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -510,38 +510,39 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>